<commit_message>
New Project for CRM
</commit_message>
<xml_diff>
--- a/CRM Project/crm/reporting.xlsx
+++ b/CRM Project/crm/reporting.xlsx
@@ -27,55 +27,55 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>fsdsdfsf</t>
+  </si>
+  <si>
+    <t>mahendrawe</t>
+  </si>
+  <si>
+    <t>zxccxz</t>
+  </si>
+  <si>
+    <t>zcxccz</t>
+  </si>
+  <si>
+    <t>zcxzcz</t>
+  </si>
+  <si>
+    <t>zczc</t>
+  </si>
+  <si>
+    <t>zxczcxczxc</t>
+  </si>
+  <si>
+    <t>ddsds</t>
+  </si>
+  <si>
+    <t>atul khandar</t>
+  </si>
+  <si>
+    <t>sfdvfsdd</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>sddfvsdfs</t>
+  </si>
+  <si>
     <t>Remarks</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>Sr. No.</t>
-  </si>
-  <si>
-    <t>call</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>fsdsdfsf</t>
-  </si>
-  <si>
-    <t>mahendrawe</t>
-  </si>
-  <si>
-    <t>zxccxz</t>
-  </si>
-  <si>
-    <t>zcxccz</t>
-  </si>
-  <si>
-    <t>zcxzcz</t>
-  </si>
-  <si>
-    <t>zczc</t>
-  </si>
-  <si>
-    <t>zxczcxczxc</t>
-  </si>
-  <si>
-    <t>ddsds</t>
-  </si>
-  <si>
-    <t>atul khandar</t>
-  </si>
-  <si>
-    <t>sfdvfsdd</t>
-  </si>
-  <si>
-    <t>sdfsd</t>
-  </si>
-  <si>
-    <t>sddfvsdfs</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,13 +460,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="37.5">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -475,7 +475,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1">
@@ -483,19 +483,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
         <v>3243</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="23.25" customHeight="1">
@@ -503,19 +503,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -523,19 +523,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>